<commit_message>
update to multiple components - mainly adding dev friendly debug logging
</commit_message>
<xml_diff>
--- a/reports/strategy_results.xlsx
+++ b/reports/strategy_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>timestamp</t>
   </si>
@@ -74,6 +74,10 @@
   </si>
   <si>
     <t xml:space="preserve">content="1️⃣ Explanation: **TSLA Intraday Momentum Reversal Strategy** - Generate 'signal' based on 5-min bar momentum: Buy if Close &gt; High of 3 periods ago &amp; RSI(10) &lt; 70, Sell if Close &lt; Low of 3 periods ago &amp; RSI(10) &gt; 30, else Hold.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content="1️⃣ Explanation: **TSLA Intraday Momentum Reversal Strategy** - Generates 'signal' based on 5-min bar momentum: Buy when price closes above the 3-period high after a 2-period downtrend, Sell when below the 3-period low after a 2-period uptrend, else Hold.
 </t>
   </si>
   <si>
@@ -98,6 +102,36 @@
     df.drop(columns=['CloseShift3', 'HighShift3', 'LowShift3', 
                       'DeltaClose', 'RSI_Period', 'Gain', 'Loss', 
                       'AvgGain', 'AvgLoss', 'RS', 'RSI'], inplace=True)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    df['Up'] = np.where(df['Close'] &gt; df['Close'].shift(1), 1, 0)
+    up_days = df['Up'].rolling(2).sum()
+    down_days = df['Up'].rolling(2).sum().apply(lambda x: 2 - x)
+    df['RecentUptrend'] = np.where(up_days == 2, 1, 0)
+    df['RecentDowntrend'] = np.where(down_days == 2, 1, 0)
+    df['High3'] = df['High'].rolling(3).max()
+    df['Low3'] = df['Low'].rolling(3).min()
+    df['signal'] = np.where((df['Close'] &gt; df['High3']) &amp; df['RecentDowntrend'], 1,
+                            np.where((df['Close'] &lt; df['Low3']) &amp; df['RecentUptrend'], -1, 0))
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    df['pct_change'] = df['Close'].pct_change().fillna(0)
+    up_days = df['pct_change'] &gt; 0
+    down_days = ~up_days
+    df['recent_uptrend'] = (up_days.shift(1)) &amp; (up_days.shift(2))
+    df['recent_downtrend'] = (down_days.shift(1)) &amp; (down_days.shift(2))
+    df['above_3high'] = df['Close'] &gt; df['High'].shift(1).rolling(3).max()
+    df['below_3low'] = df['Close'] &lt; df['Low'].shift(1).rolling(3).min()
+    df['signal'] = -1
+    df.loc[(df['recent_downtrend']) &amp; (df['above_3high']), 'signal'] = 1
+    df.loc[(df['recent_uptrend']) &amp; (df['below_3low']), 'signal'] = -1
+    df.loc[df['signal'] == -1, 'signal'] = 0
 </t>
   </si>
   <si>
@@ -466,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -533,16 +567,16 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="2">
-        <v>45791.58182560412</v>
+        <v>45791.58182560185</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -584,6 +618,230 @@
         <v>0</v>
       </c>
       <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="2">
+        <v>45791.59323685186</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>2.73</v>
+      </c>
+      <c r="I3">
+        <v>49.95</v>
+      </c>
+      <c r="J3">
+        <v>0.41</v>
+      </c>
+      <c r="K3">
+        <v>15</v>
+      </c>
+      <c r="L3">
+        <v>150</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="2">
+        <v>45791.59371015046</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="2">
+        <v>45791.60139868056</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>-0.35</v>
+      </c>
+      <c r="I5">
+        <v>-15.87</v>
+      </c>
+      <c r="J5">
+        <v>0.15</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="2">
+        <v>45791.60420985582</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>2.73</v>
+      </c>
+      <c r="I6">
+        <v>49.95</v>
+      </c>
+      <c r="J6">
+        <v>0.41</v>
+      </c>
+      <c r="K6">
+        <v>15</v>
+      </c>
+      <c r="L6">
+        <v>150</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to agent strategy
</commit_message>
<xml_diff>
--- a/reports/strategy_results.xlsx
+++ b/reports/strategy_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>timestamp</t>
   </si>
@@ -458,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -581,7 +581,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="2">
-        <v>45791.61911637864</v>
+        <v>45791.61911637732</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -632,6 +632,62 @@
         <v>0</v>
       </c>
       <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="2">
+        <v>45791.64495566366</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>-0.35</v>
+      </c>
+      <c r="I4">
+        <v>-15.87</v>
+      </c>
+      <c r="J4">
+        <v>0.15</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>0</v>
       </c>
     </row>

</xml_diff>